<commit_message>
reconstruct be and add name prop for input
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\Project\KmaManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8118AE-624C-4AD2-8965-FCD5585E28F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1E855E-64E9-4D25-8D2D-F5E035CB0ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>student</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>exercise</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -297,10 +300,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,15 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:O48"/>
+  <dimension ref="B3:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -600,26 +603,35 @@
       <c r="F3" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="K3" t="s">
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" t="s">
         <v>59</v>
-      </c>
-      <c r="L3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" t="s">
-        <v>64</v>
       </c>
       <c r="O3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="P3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -629,18 +641,27 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="4"/>
       <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" t="s">
         <v>60</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="S4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -650,18 +671,27 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="4"/>
       <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="L5" t="s">
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" t="s">
         <v>61</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="S5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -671,49 +701,67 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="4"/>
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="O6" t="s">
         <v>11</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="S6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="4"/>
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>62</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>69</v>
+      </c>
+      <c r="R7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G8" s="3"/>
+      <c r="S7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G8" s="4"/>
       <c r="H8" t="s">
         <v>14</v>
       </c>
-      <c r="L8" t="s">
+      <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
+        <v>69</v>
+      </c>
+      <c r="R8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G9" s="3"/>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G9" s="4"/>
       <c r="H9" t="s">
         <v>15</v>
       </c>
@@ -723,206 +771,230 @@
       <c r="J9" t="s">
         <v>17</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" t="s">
         <v>63</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G10" s="3"/>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G10" s="4"/>
       <c r="H10" t="s">
         <v>18</v>
       </c>
-      <c r="L10" t="s">
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="O10" t="s">
         <v>18</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>69</v>
+      </c>
+      <c r="R10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G11" s="3"/>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G11" s="4"/>
       <c r="H11" t="s">
         <v>17</v>
       </c>
-      <c r="L11" t="s">
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O11" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G12" s="4" t="s">
+      <c r="P11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G13" s="4"/>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G13" s="3"/>
       <c r="H13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G14" s="4"/>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G14" s="3"/>
       <c r="H14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G15" s="4" t="s">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G15" s="3" t="s">
         <v>55</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G16" s="4"/>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G16" s="3"/>
       <c r="H16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G17" s="4"/>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G17" s="3"/>
       <c r="H17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G18" s="4"/>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G18" s="3"/>
       <c r="H18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G19" s="4"/>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G19" s="3"/>
       <c r="H19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G20" s="4"/>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G20" s="3"/>
       <c r="H20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G21" s="4"/>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G21" s="3"/>
       <c r="H21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="7:8" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="G22" s="4"/>
+    <row r="22" spans="7:10" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="G22" s="3"/>
       <c r="H22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G23" s="4" t="s">
+    <row r="23" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G23" s="3" t="s">
         <v>56</v>
       </c>
       <c r="H23" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G24" s="4"/>
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G24" s="3"/>
       <c r="H24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G25" s="4"/>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G25" s="3"/>
       <c r="H25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G26" s="4"/>
+    <row r="26" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G26" s="3"/>
       <c r="H26" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G27" s="4"/>
+      <c r="I26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G27" s="3"/>
       <c r="H27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G28" s="4"/>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G28" s="3"/>
       <c r="H28" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G29" s="4" t="s">
+    <row r="29" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G29" s="3" t="s">
         <v>57</v>
       </c>
       <c r="H29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G30" s="4"/>
+    <row r="30" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G30" s="3"/>
       <c r="H30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G31" s="4"/>
+    <row r="31" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G31" s="3"/>
       <c r="H31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G32" s="4"/>
+    <row r="32" spans="7:10" x14ac:dyDescent="0.35">
+      <c r="G32" s="3"/>
       <c r="H32" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G33" s="4"/>
+      <c r="G33" s="3"/>
       <c r="H33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G34" s="4"/>
+      <c r="G34" s="3"/>
       <c r="H34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G35" s="4"/>
+      <c r="G35" s="3"/>
       <c r="H35" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G36" s="4"/>
+      <c r="G36" s="3"/>
       <c r="H36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="37" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G37" s="4"/>
+      <c r="G37" s="3"/>
       <c r="H37" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="38" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G38" s="4"/>
+      <c r="G38" s="3"/>
       <c r="H38" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="39" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G39" s="4"/>
+      <c r="G39" s="3"/>
       <c r="H39" t="s">
         <v>46</v>
       </c>
@@ -931,7 +1003,7 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="3" t="s">
         <v>58</v>
       </c>
       <c r="H41" t="s">
@@ -939,43 +1011,43 @@
       </c>
     </row>
     <row r="42" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G42" s="4"/>
+      <c r="G42" s="3"/>
       <c r="H42" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="43" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G43" s="4"/>
+      <c r="G43" s="3"/>
       <c r="H43" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G44" s="4"/>
+      <c r="G44" s="3"/>
       <c r="H44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G45" s="4"/>
+      <c r="G45" s="3"/>
       <c r="H45" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="46" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G46" s="4"/>
+      <c r="G46" s="3"/>
       <c r="H46" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="47" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G47" s="4"/>
+      <c r="G47" s="3"/>
       <c r="H47" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="48" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G48" s="4"/>
+      <c r="G48" s="3"/>
       <c r="H48" t="s">
         <v>54</v>
       </c>

</xml_diff>